<commit_message>
them luong thang 6
</commit_message>
<xml_diff>
--- a/Data/062018/chamcong.xlsx
+++ b/Data/062018/chamcong.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DucTn\Desktop\luong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{671C6D9C-C354-4ABF-B0CC-C37AEFE6C12A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2130417C-8A5F-495B-AE0F-AA147A96C5ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,24 +430,24 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:J14"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
@@ -496,13 +496,13 @@
     </row>
     <row r="2" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>43221</v>
+        <v>43252</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -520,15 +520,15 @@
         <v>1</v>
       </c>
       <c r="I2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>43222</v>
+        <v>43253</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -552,15 +552,15 @@
         <v>1</v>
       </c>
       <c r="I3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>43223</v>
+        <v>43254</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -587,12 +587,12 @@
         <v>1</v>
       </c>
       <c r="J4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>43224</v>
+        <v>43255</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -619,12 +619,12 @@
         <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>43225</v>
+        <v>43256</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
@@ -651,12 +651,12 @@
         <v>1</v>
       </c>
       <c r="J6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>43226</v>
+        <v>43257</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -683,12 +683,12 @@
         <v>1</v>
       </c>
       <c r="J7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>43227</v>
+        <v>43258</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -715,12 +715,12 @@
         <v>1</v>
       </c>
       <c r="J8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>43228</v>
+        <v>43259</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5">
         <v>1</v>
@@ -744,15 +744,15 @@
         <v>1</v>
       </c>
       <c r="I9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>43229</v>
+        <v>43260</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -761,30 +761,30 @@
         <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
       </c>
       <c r="H10" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="5">
         <v>1</v>
       </c>
       <c r="J10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>43230</v>
+        <v>43261</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -796,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -811,18 +811,18 @@
         <v>1</v>
       </c>
       <c r="J11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>43231</v>
+        <v>43262</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -843,44 +843,44 @@
         <v>1</v>
       </c>
       <c r="J12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>43232</v>
+        <v>43263</v>
       </c>
       <c r="B13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>43233</v>
+        <v>43264</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="5">
         <v>1</v>
@@ -912,222 +912,550 @@
     </row>
     <row r="15" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>43234</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+        <v>43265</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>43235</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+        <v>43266</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>43236</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+        <v>43267</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>43237</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+        <v>43268</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>43238</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+        <v>43269</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>43239</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+        <v>43270</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>43240</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+        <v>43271</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>43241</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+        <v>43272</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>43242</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+        <v>43273</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>43243</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+        <v>43274</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>43244</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+        <v>43275</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>43245</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+        <v>43276</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>43246</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+        <v>43277</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>43247</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+        <v>43278</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>43248</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+        <v>43279</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>43249</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+        <v>43280</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>43250</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+        <v>43281</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>43251</v>
-      </c>
+      <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>

</xml_diff>